<commit_message>
crud operation /Admin/Staff Management feature done
</commit_message>
<xml_diff>
--- a/data/userInfo.xlsx
+++ b/data/userInfo.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
   <si>
     <t>userName</t>
   </si>
@@ -22,7 +22,19 @@
     <t>userPass</t>
   </si>
   <si>
+    <t>userRole</t>
+  </si>
+  <si>
     <t>admin</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>role</t>
   </si>
 </sst>
 </file>
@@ -332,26 +344,43 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>